<commit_message>
Activity Bar Chart Update
</commit_message>
<xml_diff>
--- a/Activity Bar Chart.xlsx
+++ b/Activity Bar Chart.xlsx
@@ -1,34 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Huy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E8263BE-018D-4567-A173-6C16AA099059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4CA899-6934-45D1-8D82-FE2167FB41F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
     <sheet name="About" sheetId="12" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">ProjectSchedule!$4:$6</definedName>
     <definedName name="task_end" localSheetId="0">ProjectSchedule!$F1</definedName>
     <definedName name="task_progress" localSheetId="0">ProjectSchedule!$D1</definedName>
     <definedName name="task_start" localSheetId="0">ProjectSchedule!$E1</definedName>
     <definedName name="today" localSheetId="0">ProjectSchedule!$E$3</definedName>
     <definedName name="valuevx">42.314159</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$15</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -176,9 +185,6 @@
     <t>Form sửa trạng thái mượn, trả sách</t>
   </si>
   <si>
-    <t>Tạo database bằng Migration</t>
-  </si>
-  <si>
     <t>Form Thêm, sửa, xóa nhân viên</t>
   </si>
   <si>
@@ -228,6 +234,9 @@
   </si>
   <si>
     <t>Form thống kê tình trạng sách(còn,mượn,trễ hẹn)</t>
+  </si>
+  <si>
+    <t>Tạo database</t>
   </si>
 </sst>
 </file>
@@ -915,109 +924,109 @@
     <xf numFmtId="167" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="6" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="24" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="25" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="26" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="24" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="25" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="26" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Calculation" xfId="5" builtinId="22"/>
-    <cellStyle name="Good" xfId="3" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Phần trăm" xfId="2" builtinId="5"/>
+    <cellStyle name="Siêu kết nối" xfId="1" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Tính toán" xfId="5" builtinId="22"/>
+    <cellStyle name="Tốt" xfId="3" builtinId="26"/>
+    <cellStyle name="Trung lập" xfId="4" builtinId="28"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -1569,11 +1578,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BK60"/>
+  <dimension ref="A1:BR60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BL3" sqref="BL3"/>
+      <selection pane="bottomLeft" activeCell="BL9" sqref="BL9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,149 +1595,162 @@
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="2.7109375" customWidth="1"/>
     <col min="8" max="63" width="2.5703125" customWidth="1"/>
-    <col min="68" max="69" width="10.28515625"/>
+    <col min="64" max="64" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="1.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B1" s="74" t="s">
+    <row r="1" spans="1:70" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="74"/>
+      <c r="C1" s="43"/>
       <c r="D1" s="21"/>
       <c r="E1" s="2"/>
       <c r="F1" s="32"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-    </row>
-    <row r="2" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="42" t="s">
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="74"/>
+      <c r="Z1" s="74"/>
+    </row>
+    <row r="2" spans="1:70" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="42"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="40">
+      <c r="E2" s="69">
         <v>44113</v>
       </c>
-      <c r="F2" s="41"/>
-    </row>
-    <row r="3" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="70"/>
+    </row>
+    <row r="3" spans="1:70" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7"/>
       <c r="D3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="40">
-        <v>44114</v>
-      </c>
-      <c r="F3" s="41"/>
-    </row>
-    <row r="4" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="69">
+        <v>44170</v>
+      </c>
+      <c r="F3" s="70"/>
+    </row>
+    <row r="4" spans="1:70" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="H4" s="37">
+      <c r="H4" s="71">
         <f>H5</f>
         <v>44109</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="37">
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="71">
         <f>O5</f>
         <v>44116</v>
       </c>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="39"/>
-      <c r="V4" s="37">
+      <c r="P4" s="72"/>
+      <c r="Q4" s="72"/>
+      <c r="R4" s="72"/>
+      <c r="S4" s="72"/>
+      <c r="T4" s="72"/>
+      <c r="U4" s="73"/>
+      <c r="V4" s="71">
         <f>V5</f>
         <v>44123</v>
       </c>
-      <c r="W4" s="38"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="39"/>
-      <c r="AC4" s="37">
+      <c r="W4" s="72"/>
+      <c r="X4" s="72"/>
+      <c r="Y4" s="72"/>
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72"/>
+      <c r="AB4" s="73"/>
+      <c r="AC4" s="71">
         <f>AC5</f>
         <v>44130</v>
       </c>
-      <c r="AD4" s="38"/>
-      <c r="AE4" s="38"/>
-      <c r="AF4" s="38"/>
-      <c r="AG4" s="38"/>
-      <c r="AH4" s="38"/>
-      <c r="AI4" s="39"/>
-      <c r="AJ4" s="37">
+      <c r="AD4" s="72"/>
+      <c r="AE4" s="72"/>
+      <c r="AF4" s="72"/>
+      <c r="AG4" s="72"/>
+      <c r="AH4" s="72"/>
+      <c r="AI4" s="73"/>
+      <c r="AJ4" s="71">
         <f>AJ5</f>
         <v>44137</v>
       </c>
-      <c r="AK4" s="38"/>
-      <c r="AL4" s="38"/>
-      <c r="AM4" s="38"/>
-      <c r="AN4" s="38"/>
-      <c r="AO4" s="38"/>
-      <c r="AP4" s="39"/>
-      <c r="AQ4" s="37">
+      <c r="AK4" s="72"/>
+      <c r="AL4" s="72"/>
+      <c r="AM4" s="72"/>
+      <c r="AN4" s="72"/>
+      <c r="AO4" s="72"/>
+      <c r="AP4" s="73"/>
+      <c r="AQ4" s="71">
         <f>AQ5</f>
         <v>44144</v>
       </c>
-      <c r="AR4" s="38"/>
-      <c r="AS4" s="38"/>
-      <c r="AT4" s="38"/>
-      <c r="AU4" s="38"/>
-      <c r="AV4" s="38"/>
-      <c r="AW4" s="39"/>
-      <c r="AX4" s="37">
+      <c r="AR4" s="72"/>
+      <c r="AS4" s="72"/>
+      <c r="AT4" s="72"/>
+      <c r="AU4" s="72"/>
+      <c r="AV4" s="72"/>
+      <c r="AW4" s="73"/>
+      <c r="AX4" s="71">
         <f>AX5</f>
         <v>44151</v>
       </c>
-      <c r="AY4" s="38"/>
-      <c r="AZ4" s="38"/>
-      <c r="BA4" s="38"/>
-      <c r="BB4" s="38"/>
-      <c r="BC4" s="38"/>
-      <c r="BD4" s="39"/>
-      <c r="BE4" s="37">
+      <c r="AY4" s="72"/>
+      <c r="AZ4" s="72"/>
+      <c r="BA4" s="72"/>
+      <c r="BB4" s="72"/>
+      <c r="BC4" s="72"/>
+      <c r="BD4" s="73"/>
+      <c r="BE4" s="71">
         <f>BE5</f>
         <v>44158</v>
       </c>
-      <c r="BF4" s="38"/>
-      <c r="BG4" s="38"/>
-      <c r="BH4" s="38"/>
-      <c r="BI4" s="38"/>
-      <c r="BJ4" s="38"/>
-      <c r="BK4" s="39"/>
-    </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="BF4" s="72"/>
+      <c r="BG4" s="72"/>
+      <c r="BH4" s="72"/>
+      <c r="BI4" s="72"/>
+      <c r="BJ4" s="72"/>
+      <c r="BK4" s="73"/>
+      <c r="BL4" s="71">
+        <f>BL5</f>
+        <v>44165</v>
+      </c>
+      <c r="BM4" s="72"/>
+      <c r="BN4" s="72"/>
+      <c r="BO4" s="72"/>
+      <c r="BP4" s="72"/>
+      <c r="BQ4" s="72"/>
+      <c r="BR4" s="73"/>
+    </row>
+    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="11">
@@ -1955,8 +1977,36 @@
         <f t="shared" si="2"/>
         <v>44164</v>
       </c>
-    </row>
-    <row r="6" spans="1:63" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL5" s="11">
+        <f>BK5+1</f>
+        <v>44165</v>
+      </c>
+      <c r="BM5" s="10">
+        <f>BL5+1</f>
+        <v>44166</v>
+      </c>
+      <c r="BN5" s="10">
+        <f t="shared" ref="BN5" si="3">BM5+1</f>
+        <v>44167</v>
+      </c>
+      <c r="BO5" s="10">
+        <f t="shared" ref="BO5" si="4">BN5+1</f>
+        <v>44168</v>
+      </c>
+      <c r="BP5" s="10">
+        <f t="shared" ref="BP5" si="5">BO5+1</f>
+        <v>44169</v>
+      </c>
+      <c r="BQ5" s="10">
+        <f t="shared" ref="BQ5" si="6">BP5+1</f>
+        <v>44170</v>
+      </c>
+      <c r="BR5" s="12">
+        <f t="shared" ref="BR5" si="7">BQ5+1</f>
+        <v>44171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:70" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="8" t="s">
         <v>11</v>
@@ -1968,236 +2018,264 @@
       <c r="E6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="47"/>
+      <c r="G6" s="59"/>
       <c r="H6" s="13" t="str">
-        <f t="shared" ref="H6" si="3">LEFT(TEXT(H5,"ddd"),1)</f>
+        <f t="shared" ref="H6" si="8">LEFT(TEXT(H5,"ddd"),1)</f>
         <v>M</v>
       </c>
       <c r="I6" s="13" t="str">
-        <f t="shared" ref="I6:AQ6" si="4">LEFT(TEXT(I5,"ddd"),1)</f>
+        <f t="shared" ref="I6:AQ6" si="9">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="J6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>W</v>
       </c>
       <c r="K6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
       <c r="L6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>F</v>
       </c>
       <c r="M6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
       <c r="N6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
       <c r="O6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>M</v>
       </c>
       <c r="P6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
       <c r="Q6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>W</v>
       </c>
       <c r="R6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
       <c r="S6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>F</v>
       </c>
       <c r="T6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
       <c r="U6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
       <c r="V6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>M</v>
       </c>
       <c r="W6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
       <c r="X6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>W</v>
       </c>
       <c r="Y6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
       <c r="Z6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>F</v>
       </c>
       <c r="AA6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
       <c r="AB6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
       <c r="AC6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>M</v>
       </c>
       <c r="AD6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
       <c r="AE6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>W</v>
       </c>
       <c r="AF6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
       <c r="AG6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>F</v>
       </c>
       <c r="AH6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
       <c r="AI6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
       <c r="AJ6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>M</v>
       </c>
       <c r="AK6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
       <c r="AL6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>W</v>
       </c>
       <c r="AM6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
       <c r="AN6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>F</v>
       </c>
       <c r="AO6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
       <c r="AP6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
       <c r="AQ6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>M</v>
       </c>
       <c r="AR6" s="13" t="str">
-        <f t="shared" ref="AR6:BK6" si="5">LEFT(TEXT(AR5,"ddd"),1)</f>
+        <f t="shared" ref="AR6:BL6" si="10">LEFT(TEXT(AR5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="AS6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>W</v>
       </c>
       <c r="AT6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>T</v>
       </c>
       <c r="AU6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>F</v>
       </c>
       <c r="AV6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
       <c r="AW6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
       <c r="AX6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="AY6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>T</v>
       </c>
       <c r="AZ6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>W</v>
       </c>
       <c r="BA6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>T</v>
       </c>
       <c r="BB6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>F</v>
       </c>
       <c r="BC6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
       <c r="BD6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
       <c r="BE6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
       <c r="BF6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>T</v>
       </c>
       <c r="BG6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>W</v>
       </c>
       <c r="BH6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>T</v>
       </c>
       <c r="BI6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>F</v>
       </c>
       <c r="BJ6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
       <c r="BK6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="7" spans="1:63" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL6" s="13" t="str">
+        <f t="shared" ref="BL6:BR6" si="11">LEFT(TEXT(BL5,"ddd"),1)</f>
+        <v>M</v>
+      </c>
+      <c r="BM6" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v>T</v>
+      </c>
+      <c r="BN6" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v>W</v>
+      </c>
+      <c r="BO6" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v>T</v>
+      </c>
+      <c r="BP6" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v>F</v>
+      </c>
+      <c r="BQ6" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v>S</v>
+      </c>
+      <c r="BR6" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="7" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="15" t="s">
         <v>3</v>
@@ -2207,10 +2285,10 @@
       <c r="E7" s="35">
         <v>44113</v>
       </c>
-      <c r="F7" s="48">
+      <c r="F7" s="53">
         <v>44113</v>
       </c>
-      <c r="G7" s="49"/>
+      <c r="G7" s="54"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
@@ -2267,8 +2345,15 @@
       <c r="BI7" s="18"/>
       <c r="BJ7" s="18"/>
       <c r="BK7" s="18"/>
-    </row>
-    <row r="8" spans="1:63" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL7" s="18"/>
+      <c r="BM7" s="18"/>
+      <c r="BN7" s="18"/>
+      <c r="BO7" s="18"/>
+      <c r="BP7" s="18"/>
+      <c r="BQ7" s="18"/>
+      <c r="BR7" s="18"/>
+    </row>
+    <row r="8" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="15" t="s">
         <v>4</v>
@@ -2278,10 +2363,10 @@
       <c r="E8" s="35">
         <v>44113</v>
       </c>
-      <c r="F8" s="48">
+      <c r="F8" s="53">
         <v>44114</v>
       </c>
-      <c r="G8" s="49"/>
+      <c r="G8" s="54"/>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
@@ -2338,17 +2423,28 @@
       <c r="BI8" s="18"/>
       <c r="BJ8" s="18"/>
       <c r="BK8" s="18"/>
-    </row>
-    <row r="9" spans="1:63" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL8" s="18"/>
+      <c r="BM8" s="18"/>
+      <c r="BN8" s="18"/>
+      <c r="BO8" s="18"/>
+      <c r="BP8" s="18"/>
+      <c r="BQ8" s="18"/>
+      <c r="BR8" s="18"/>
+    </row>
+    <row r="9" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="49"/>
+      <c r="E9" s="35">
+        <v>44169</v>
+      </c>
+      <c r="F9" s="53">
+        <v>44170</v>
+      </c>
+      <c r="G9" s="54"/>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
@@ -2405,17 +2501,28 @@
       <c r="BI9" s="18"/>
       <c r="BJ9" s="18"/>
       <c r="BK9" s="18"/>
-    </row>
-    <row r="10" spans="1:63" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL9" s="18"/>
+      <c r="BM9" s="18"/>
+      <c r="BN9" s="18"/>
+      <c r="BO9" s="18"/>
+      <c r="BP9" s="18"/>
+      <c r="BQ9" s="18"/>
+      <c r="BR9" s="18"/>
+    </row>
+    <row r="10" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="49"/>
+      <c r="E10" s="35">
+        <v>44169</v>
+      </c>
+      <c r="F10" s="53">
+        <v>44170</v>
+      </c>
+      <c r="G10" s="54"/>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
@@ -2472,17 +2579,28 @@
       <c r="BI10" s="18"/>
       <c r="BJ10" s="18"/>
       <c r="BK10" s="18"/>
-    </row>
-    <row r="11" spans="1:63" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL10" s="18"/>
+      <c r="BM10" s="18"/>
+      <c r="BN10" s="18"/>
+      <c r="BO10" s="18"/>
+      <c r="BP10" s="18"/>
+      <c r="BQ10" s="18"/>
+      <c r="BR10" s="18"/>
+    </row>
+    <row r="11" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="49"/>
+      <c r="E11" s="35">
+        <v>44169</v>
+      </c>
+      <c r="F11" s="53">
+        <v>44170</v>
+      </c>
+      <c r="G11" s="54"/>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
@@ -2539,17 +2657,28 @@
       <c r="BI11" s="18"/>
       <c r="BJ11" s="18"/>
       <c r="BK11" s="18"/>
-    </row>
-    <row r="12" spans="1:63" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL11" s="18"/>
+      <c r="BM11" s="18"/>
+      <c r="BN11" s="18"/>
+      <c r="BO11" s="18"/>
+      <c r="BP11" s="18"/>
+      <c r="BQ11" s="18"/>
+      <c r="BR11" s="18"/>
+    </row>
+    <row r="12" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="17"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="49"/>
+      <c r="E12" s="35">
+        <v>44169</v>
+      </c>
+      <c r="F12" s="53">
+        <v>44170</v>
+      </c>
+      <c r="G12" s="54"/>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
@@ -2606,17 +2735,28 @@
       <c r="BI12" s="18"/>
       <c r="BJ12" s="18"/>
       <c r="BK12" s="18"/>
-    </row>
-    <row r="13" spans="1:63" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL12" s="18"/>
+      <c r="BM12" s="18"/>
+      <c r="BN12" s="18"/>
+      <c r="BO12" s="18"/>
+      <c r="BP12" s="18"/>
+      <c r="BQ12" s="18"/>
+      <c r="BR12" s="18"/>
+    </row>
+    <row r="13" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="17"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="49"/>
+      <c r="E13" s="35">
+        <v>44169</v>
+      </c>
+      <c r="F13" s="53">
+        <v>44170</v>
+      </c>
+      <c r="G13" s="54"/>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
@@ -2673,17 +2813,28 @@
       <c r="BI13" s="18"/>
       <c r="BJ13" s="18"/>
       <c r="BK13" s="18"/>
-    </row>
-    <row r="14" spans="1:63" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL13" s="18"/>
+      <c r="BM13" s="18"/>
+      <c r="BN13" s="18"/>
+      <c r="BO13" s="18"/>
+      <c r="BP13" s="18"/>
+      <c r="BQ13" s="18"/>
+      <c r="BR13" s="18"/>
+    </row>
+    <row r="14" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="17"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="49"/>
+      <c r="E14" s="35">
+        <v>44169</v>
+      </c>
+      <c r="F14" s="53">
+        <v>44170</v>
+      </c>
+      <c r="G14" s="54"/>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
@@ -2740,17 +2891,28 @@
       <c r="BI14" s="18"/>
       <c r="BJ14" s="18"/>
       <c r="BK14" s="18"/>
-    </row>
-    <row r="15" spans="1:63" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL14" s="18"/>
+      <c r="BM14" s="18"/>
+      <c r="BN14" s="18"/>
+      <c r="BO14" s="18"/>
+      <c r="BP14" s="18"/>
+      <c r="BQ14" s="18"/>
+      <c r="BR14" s="18"/>
+    </row>
+    <row r="15" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="17"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
+      <c r="E15" s="35">
+        <v>44169</v>
+      </c>
+      <c r="F15" s="53">
+        <v>44170</v>
+      </c>
+      <c r="G15" s="54"/>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
@@ -2807,17 +2969,28 @@
       <c r="BI15" s="18"/>
       <c r="BJ15" s="18"/>
       <c r="BK15" s="18"/>
-    </row>
-    <row r="16" spans="1:63" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL15" s="18"/>
+      <c r="BM15" s="18"/>
+      <c r="BN15" s="18"/>
+      <c r="BO15" s="18"/>
+      <c r="BP15" s="18"/>
+      <c r="BQ15" s="18"/>
+      <c r="BR15" s="18"/>
+    </row>
+    <row r="16" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="17"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="49"/>
+      <c r="E16" s="35">
+        <v>44169</v>
+      </c>
+      <c r="F16" s="53">
+        <v>44170</v>
+      </c>
+      <c r="G16" s="54"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
@@ -2874,17 +3047,28 @@
       <c r="BI16" s="18"/>
       <c r="BJ16" s="18"/>
       <c r="BK16" s="18"/>
-    </row>
-    <row r="17" spans="1:63" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL16" s="18"/>
+      <c r="BM16" s="18"/>
+      <c r="BN16" s="18"/>
+      <c r="BO16" s="18"/>
+      <c r="BP16" s="18"/>
+      <c r="BQ16" s="18"/>
+      <c r="BR16" s="18"/>
+    </row>
+    <row r="17" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="17"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="49"/>
+      <c r="E17" s="35">
+        <v>44169</v>
+      </c>
+      <c r="F17" s="53">
+        <v>44170</v>
+      </c>
+      <c r="G17" s="54"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
@@ -2941,17 +3125,28 @@
       <c r="BI17" s="18"/>
       <c r="BJ17" s="18"/>
       <c r="BK17" s="18"/>
-    </row>
-    <row r="18" spans="1:63" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL17" s="18"/>
+      <c r="BM17" s="18"/>
+      <c r="BN17" s="18"/>
+      <c r="BO17" s="18"/>
+      <c r="BP17" s="18"/>
+      <c r="BQ17" s="18"/>
+      <c r="BR17" s="18"/>
+    </row>
+    <row r="18" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="17"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="49"/>
+      <c r="E18" s="35">
+        <v>44169</v>
+      </c>
+      <c r="F18" s="53">
+        <v>44170</v>
+      </c>
+      <c r="G18" s="54"/>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
@@ -3008,17 +3203,28 @@
       <c r="BI18" s="18"/>
       <c r="BJ18" s="18"/>
       <c r="BK18" s="18"/>
-    </row>
-    <row r="19" spans="1:63" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL18" s="18"/>
+      <c r="BM18" s="18"/>
+      <c r="BN18" s="18"/>
+      <c r="BO18" s="18"/>
+      <c r="BP18" s="18"/>
+      <c r="BQ18" s="18"/>
+      <c r="BR18" s="18"/>
+    </row>
+    <row r="19" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="17"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="49"/>
+      <c r="E19" s="35">
+        <v>44169</v>
+      </c>
+      <c r="F19" s="53">
+        <v>44170</v>
+      </c>
+      <c r="G19" s="54"/>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
@@ -3075,696 +3281,763 @@
       <c r="BI19" s="18"/>
       <c r="BJ19" s="18"/>
       <c r="BK19" s="18"/>
-    </row>
-    <row r="21" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="43"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="43"/>
-      <c r="R21" s="43"/>
-      <c r="S21" s="43"/>
-      <c r="T21" s="43"/>
-      <c r="U21" s="43"/>
-      <c r="V21" s="43"/>
-    </row>
-    <row r="22" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="B22" s="50" t="s">
+      <c r="BL19" s="18"/>
+      <c r="BM19" s="18"/>
+      <c r="BN19" s="18"/>
+      <c r="BO19" s="18"/>
+      <c r="BP19" s="18"/>
+      <c r="BQ19" s="18"/>
+      <c r="BR19" s="18"/>
+    </row>
+    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="48"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="48"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="48"/>
+      <c r="V21" s="48"/>
+    </row>
+    <row r="22" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B22" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="53" t="s">
+      <c r="C22" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56" t="s">
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="I22" s="57"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="57"/>
-      <c r="O22" s="57"/>
-      <c r="P22" s="57"/>
-      <c r="Q22" s="57"/>
-      <c r="R22" s="57"/>
-      <c r="S22" s="57"/>
-      <c r="T22" s="57"/>
-      <c r="U22" s="57"/>
-      <c r="V22" s="58"/>
-    </row>
-    <row r="23" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="B23" s="45" t="s">
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="56"/>
+      <c r="Q22" s="56"/>
+      <c r="R22" s="56"/>
+      <c r="S22" s="56"/>
+      <c r="T22" s="56"/>
+      <c r="U22" s="56"/>
+      <c r="V22" s="57"/>
+    </row>
+    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B23" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="59" t="s">
+      <c r="C23" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="59" t="s">
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="60"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="60"/>
-      <c r="R23" s="60"/>
-      <c r="S23" s="60"/>
-      <c r="T23" s="60"/>
-      <c r="U23" s="60"/>
-      <c r="V23" s="61"/>
-    </row>
-    <row r="24" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="B24" s="45" t="s">
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="46"/>
+      <c r="S23" s="46"/>
+      <c r="T23" s="46"/>
+      <c r="U23" s="46"/>
+      <c r="V23" s="47"/>
+    </row>
+    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B24" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="59" t="s">
+      <c r="C24" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="59" t="s">
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="I24" s="60"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="60"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="60"/>
-      <c r="O24" s="60"/>
-      <c r="P24" s="60"/>
-      <c r="Q24" s="60"/>
-      <c r="R24" s="60"/>
-      <c r="S24" s="60"/>
-      <c r="T24" s="60"/>
-      <c r="U24" s="60"/>
-      <c r="V24" s="61"/>
-    </row>
-    <row r="25" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="B25" s="45" t="s">
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="46"/>
+      <c r="Q24" s="46"/>
+      <c r="R24" s="46"/>
+      <c r="S24" s="46"/>
+      <c r="T24" s="46"/>
+      <c r="U24" s="46"/>
+      <c r="V24" s="47"/>
+    </row>
+    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B25" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="59" t="s">
+      <c r="C25" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="46"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="46"/>
+      <c r="S25" s="46"/>
+      <c r="T25" s="46"/>
+      <c r="U25" s="46"/>
+      <c r="V25" s="47"/>
+    </row>
+    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B26" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="46"/>
+      <c r="O26" s="46"/>
+      <c r="P26" s="46"/>
+      <c r="Q26" s="46"/>
+      <c r="R26" s="46"/>
+      <c r="S26" s="46"/>
+      <c r="T26" s="46"/>
+      <c r="U26" s="46"/>
+      <c r="V26" s="47"/>
+    </row>
+    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B27" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="46"/>
+      <c r="P27" s="46"/>
+      <c r="Q27" s="46"/>
+      <c r="R27" s="46"/>
+      <c r="S27" s="46"/>
+      <c r="T27" s="46"/>
+      <c r="U27" s="46"/>
+      <c r="V27" s="47"/>
+    </row>
+    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B28" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="59" t="s">
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="46"/>
+      <c r="P28" s="46"/>
+      <c r="Q28" s="46"/>
+      <c r="R28" s="46"/>
+      <c r="S28" s="46"/>
+      <c r="T28" s="46"/>
+      <c r="U28" s="46"/>
+      <c r="V28" s="47"/>
+    </row>
+    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B29" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="I25" s="60"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="60"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="60"/>
-      <c r="P25" s="60"/>
-      <c r="Q25" s="60"/>
-      <c r="R25" s="60"/>
-      <c r="S25" s="60"/>
-      <c r="T25" s="60"/>
-      <c r="U25" s="60"/>
-      <c r="V25" s="61"/>
-    </row>
-    <row r="26" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="B26" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="59" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="59" t="s">
-        <v>58</v>
-      </c>
-      <c r="I26" s="60"/>
-      <c r="J26" s="60"/>
-      <c r="K26" s="60"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="60"/>
-      <c r="N26" s="60"/>
-      <c r="O26" s="60"/>
-      <c r="P26" s="60"/>
-      <c r="Q26" s="60"/>
-      <c r="R26" s="60"/>
-      <c r="S26" s="60"/>
-      <c r="T26" s="60"/>
-      <c r="U26" s="60"/>
-      <c r="V26" s="61"/>
-    </row>
-    <row r="27" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="B27" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="59" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="59" t="s">
-        <v>58</v>
-      </c>
-      <c r="I27" s="60"/>
-      <c r="J27" s="60"/>
-      <c r="K27" s="60"/>
-      <c r="L27" s="60"/>
-      <c r="M27" s="60"/>
-      <c r="N27" s="60"/>
-      <c r="O27" s="60"/>
-      <c r="P27" s="60"/>
-      <c r="Q27" s="60"/>
-      <c r="R27" s="60"/>
-      <c r="S27" s="60"/>
-      <c r="T27" s="60"/>
-      <c r="U27" s="60"/>
-      <c r="V27" s="61"/>
-    </row>
-    <row r="28" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="B28" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="59" t="s">
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="46"/>
+      <c r="P29" s="46"/>
+      <c r="Q29" s="46"/>
+      <c r="R29" s="46"/>
+      <c r="S29" s="46"/>
+      <c r="T29" s="46"/>
+      <c r="U29" s="46"/>
+      <c r="V29" s="47"/>
+    </row>
+    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B30" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="I28" s="60"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="60"/>
-      <c r="M28" s="60"/>
-      <c r="N28" s="60"/>
-      <c r="O28" s="60"/>
-      <c r="P28" s="60"/>
-      <c r="Q28" s="60"/>
-      <c r="R28" s="60"/>
-      <c r="S28" s="60"/>
-      <c r="T28" s="60"/>
-      <c r="U28" s="60"/>
-      <c r="V28" s="61"/>
-    </row>
-    <row r="29" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="B29" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="I29" s="60"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="60"/>
-      <c r="M29" s="60"/>
-      <c r="N29" s="60"/>
-      <c r="O29" s="60"/>
-      <c r="P29" s="60"/>
-      <c r="Q29" s="60"/>
-      <c r="R29" s="60"/>
-      <c r="S29" s="60"/>
-      <c r="T29" s="60"/>
-      <c r="U29" s="60"/>
-      <c r="V29" s="61"/>
-    </row>
-    <row r="30" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="B30" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="59" t="s">
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="46"/>
+      <c r="O30" s="46"/>
+      <c r="P30" s="46"/>
+      <c r="Q30" s="46"/>
+      <c r="R30" s="46"/>
+      <c r="S30" s="46"/>
+      <c r="T30" s="46"/>
+      <c r="U30" s="46"/>
+      <c r="V30" s="47"/>
+    </row>
+    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B31" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="60"/>
-      <c r="M30" s="60"/>
-      <c r="N30" s="60"/>
-      <c r="O30" s="60"/>
-      <c r="P30" s="60"/>
-      <c r="Q30" s="60"/>
-      <c r="R30" s="60"/>
-      <c r="S30" s="60"/>
-      <c r="T30" s="60"/>
-      <c r="U30" s="60"/>
-      <c r="V30" s="61"/>
-    </row>
-    <row r="31" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="B31" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="59" t="s">
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="46"/>
+      <c r="R31" s="46"/>
+      <c r="S31" s="46"/>
+      <c r="T31" s="46"/>
+      <c r="U31" s="46"/>
+      <c r="V31" s="47"/>
+    </row>
+    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B32" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="I31" s="60"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="60"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="60"/>
-      <c r="N31" s="60"/>
-      <c r="O31" s="60"/>
-      <c r="P31" s="60"/>
-      <c r="Q31" s="60"/>
-      <c r="R31" s="60"/>
-      <c r="S31" s="60"/>
-      <c r="T31" s="60"/>
-      <c r="U31" s="60"/>
-      <c r="V31" s="61"/>
-    </row>
-    <row r="32" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="B32" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="I32" s="60"/>
-      <c r="J32" s="60"/>
-      <c r="K32" s="60"/>
-      <c r="L32" s="60"/>
-      <c r="M32" s="60"/>
-      <c r="N32" s="60"/>
-      <c r="O32" s="60"/>
-      <c r="P32" s="60"/>
-      <c r="Q32" s="60"/>
-      <c r="R32" s="60"/>
-      <c r="S32" s="60"/>
-      <c r="T32" s="60"/>
-      <c r="U32" s="60"/>
-      <c r="V32" s="61"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="46"/>
+      <c r="P32" s="46"/>
+      <c r="Q32" s="46"/>
+      <c r="R32" s="46"/>
+      <c r="S32" s="46"/>
+      <c r="T32" s="46"/>
+      <c r="U32" s="46"/>
+      <c r="V32" s="47"/>
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B33" s="45" t="s">
+      <c r="B33" s="38" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" s="64"/>
       <c r="E33" s="64"/>
       <c r="F33" s="64"/>
       <c r="G33" s="65"/>
-      <c r="H33" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="I33" s="60"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="60"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="60"/>
-      <c r="N33" s="60"/>
-      <c r="O33" s="60"/>
-      <c r="P33" s="60"/>
-      <c r="Q33" s="60"/>
-      <c r="R33" s="60"/>
-      <c r="S33" s="60"/>
-      <c r="T33" s="60"/>
-      <c r="U33" s="60"/>
-      <c r="V33" s="61"/>
+      <c r="H33" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="46"/>
+      <c r="P33" s="46"/>
+      <c r="Q33" s="46"/>
+      <c r="R33" s="46"/>
+      <c r="S33" s="46"/>
+      <c r="T33" s="46"/>
+      <c r="U33" s="46"/>
+      <c r="V33" s="47"/>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B34" s="66" t="s">
+      <c r="B34" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="67" t="s">
+      <c r="C34" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="70" t="s">
-        <v>54</v>
-      </c>
-      <c r="I34" s="71"/>
-      <c r="J34" s="71"/>
-      <c r="K34" s="71"/>
-      <c r="L34" s="71"/>
-      <c r="M34" s="71"/>
-      <c r="N34" s="71"/>
-      <c r="O34" s="71"/>
-      <c r="P34" s="71"/>
-      <c r="Q34" s="71"/>
-      <c r="R34" s="71"/>
-      <c r="S34" s="71"/>
-      <c r="T34" s="71"/>
-      <c r="U34" s="71"/>
-      <c r="V34" s="72"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
+      <c r="L34" s="61"/>
+      <c r="M34" s="61"/>
+      <c r="N34" s="61"/>
+      <c r="O34" s="61"/>
+      <c r="P34" s="61"/>
+      <c r="Q34" s="61"/>
+      <c r="R34" s="61"/>
+      <c r="S34" s="61"/>
+      <c r="T34" s="61"/>
+      <c r="U34" s="61"/>
+      <c r="V34" s="62"/>
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="73" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="73" t="s">
+      <c r="C35" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="I35" s="73"/>
-      <c r="J35" s="73"/>
-      <c r="K35" s="73"/>
-      <c r="L35" s="73"/>
-      <c r="M35" s="73"/>
-      <c r="N35" s="73"/>
-      <c r="O35" s="73"/>
-      <c r="P35" s="73"/>
-      <c r="Q35" s="73"/>
-      <c r="R35" s="73"/>
-      <c r="S35" s="73"/>
-      <c r="T35" s="73"/>
-      <c r="U35" s="73"/>
-      <c r="V35" s="73"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="52"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="52"/>
+      <c r="O35" s="52"/>
+      <c r="P35" s="52"/>
+      <c r="Q35" s="52"/>
+      <c r="R35" s="52"/>
+      <c r="S35" s="52"/>
+      <c r="T35" s="52"/>
+      <c r="U35" s="52"/>
+      <c r="V35" s="52"/>
     </row>
     <row r="36" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B37" s="50" t="s">
+      <c r="B37" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="55"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="51"/>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B38" s="44">
+      <c r="B38" s="37">
         <v>3118410148</v>
       </c>
-      <c r="C38" s="59" t="s">
+      <c r="C38" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="61"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="47"/>
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B39" s="44">
+      <c r="B39" s="37">
         <v>3118410411</v>
       </c>
-      <c r="C39" s="59" t="s">
+      <c r="C39" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="61"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="47"/>
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B40" s="44">
+      <c r="B40" s="37">
         <v>3118410188</v>
       </c>
-      <c r="C40" s="59" t="s">
+      <c r="C40" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="44"/>
+      <c r="L40" s="44"/>
+      <c r="M40" s="44"/>
+      <c r="N40" s="44"/>
+      <c r="O40" s="44"/>
+      <c r="P40" s="44"/>
+      <c r="Q40" s="44"/>
+      <c r="R40" s="44"/>
+      <c r="S40" s="44"/>
+      <c r="T40" s="44"/>
+      <c r="U40" s="44"/>
+      <c r="V40" s="44"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B41" s="37">
+        <v>3118412034</v>
+      </c>
+      <c r="C41" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="44"/>
+      <c r="L41" s="44"/>
+      <c r="M41" s="44"/>
+      <c r="N41" s="44"/>
+      <c r="O41" s="44"/>
+      <c r="P41" s="44"/>
+      <c r="Q41" s="44"/>
+      <c r="R41" s="44"/>
+      <c r="S41" s="44"/>
+      <c r="T41" s="44"/>
+      <c r="U41" s="44"/>
+      <c r="V41" s="44"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B42" s="37">
+        <v>3118410462</v>
+      </c>
+      <c r="C42" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="52"/>
-      <c r="J40" s="52"/>
-      <c r="K40" s="52"/>
-      <c r="L40" s="52"/>
-      <c r="M40" s="52"/>
-      <c r="N40" s="52"/>
-      <c r="O40" s="52"/>
-      <c r="P40" s="52"/>
-      <c r="Q40" s="52"/>
-      <c r="R40" s="52"/>
-      <c r="S40" s="52"/>
-      <c r="T40" s="52"/>
-      <c r="U40" s="52"/>
-      <c r="V40" s="52"/>
-    </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B41" s="44">
-        <v>3118412034</v>
-      </c>
-      <c r="C41" s="59" t="s">
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44"/>
+      <c r="O42" s="44"/>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="44"/>
+      <c r="R42" s="44"/>
+      <c r="S42" s="44"/>
+      <c r="T42" s="44"/>
+      <c r="U42" s="44"/>
+      <c r="V42" s="44"/>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B43" s="37">
+        <v>3118412036</v>
+      </c>
+      <c r="C43" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="52"/>
-      <c r="I41" s="52"/>
-      <c r="J41" s="52"/>
-      <c r="K41" s="52"/>
-      <c r="L41" s="52"/>
-      <c r="M41" s="52"/>
-      <c r="N41" s="52"/>
-      <c r="O41" s="52"/>
-      <c r="P41" s="52"/>
-      <c r="Q41" s="52"/>
-      <c r="R41" s="52"/>
-      <c r="S41" s="52"/>
-      <c r="T41" s="52"/>
-      <c r="U41" s="52"/>
-      <c r="V41" s="52"/>
-    </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B42" s="44">
-        <v>3118410462</v>
-      </c>
-      <c r="C42" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="52"/>
-      <c r="I42" s="52"/>
-      <c r="J42" s="52"/>
-      <c r="K42" s="52"/>
-      <c r="L42" s="52"/>
-      <c r="M42" s="52"/>
-      <c r="N42" s="52"/>
-      <c r="O42" s="52"/>
-      <c r="P42" s="52"/>
-      <c r="Q42" s="52"/>
-      <c r="R42" s="52"/>
-      <c r="S42" s="52"/>
-      <c r="T42" s="52"/>
-      <c r="U42" s="52"/>
-      <c r="V42" s="52"/>
-    </row>
-    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B43" s="44">
-        <v>3118412036</v>
-      </c>
-      <c r="C43" s="73" t="s">
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44"/>
+      <c r="O43" s="44"/>
+      <c r="P43" s="44"/>
+      <c r="Q43" s="44"/>
+      <c r="R43" s="44"/>
+      <c r="S43" s="44"/>
+      <c r="T43" s="44"/>
+      <c r="U43" s="44"/>
+      <c r="V43" s="44"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B44" s="37">
+        <v>3118410407</v>
+      </c>
+      <c r="C44" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="D43" s="73"/>
-      <c r="E43" s="73"/>
-      <c r="F43" s="73"/>
-      <c r="G43" s="73"/>
-      <c r="H43" s="52"/>
-      <c r="I43" s="52"/>
-      <c r="J43" s="52"/>
-      <c r="K43" s="52"/>
-      <c r="L43" s="52"/>
-      <c r="M43" s="52"/>
-      <c r="N43" s="52"/>
-      <c r="O43" s="52"/>
-      <c r="P43" s="52"/>
-      <c r="Q43" s="52"/>
-      <c r="R43" s="52"/>
-      <c r="S43" s="52"/>
-      <c r="T43" s="52"/>
-      <c r="U43" s="52"/>
-      <c r="V43" s="52"/>
-    </row>
-    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B44" s="44">
-        <v>3118410407</v>
-      </c>
-      <c r="C44" s="73" t="s">
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="44"/>
+      <c r="J44" s="44"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="44"/>
+      <c r="M44" s="44"/>
+      <c r="N44" s="44"/>
+      <c r="O44" s="44"/>
+      <c r="P44" s="44"/>
+      <c r="Q44" s="44"/>
+      <c r="R44" s="44"/>
+      <c r="S44" s="44"/>
+      <c r="T44" s="44"/>
+      <c r="U44" s="44"/>
+      <c r="V44" s="44"/>
+    </row>
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B45" s="37">
+        <v>3118410397</v>
+      </c>
+      <c r="C45" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="D44" s="73"/>
-      <c r="E44" s="73"/>
-      <c r="F44" s="73"/>
-      <c r="G44" s="73"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
-      <c r="K44" s="52"/>
-      <c r="L44" s="52"/>
-      <c r="M44" s="52"/>
-      <c r="N44" s="52"/>
-      <c r="O44" s="52"/>
-      <c r="P44" s="52"/>
-      <c r="Q44" s="52"/>
-      <c r="R44" s="52"/>
-      <c r="S44" s="52"/>
-      <c r="T44" s="52"/>
-      <c r="U44" s="52"/>
-      <c r="V44" s="52"/>
-    </row>
-    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B45" s="44">
-        <v>3118410397</v>
-      </c>
-      <c r="C45" s="73" t="s">
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="52"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="44"/>
+      <c r="I45" s="44"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="44"/>
+      <c r="M45" s="44"/>
+      <c r="N45" s="44"/>
+      <c r="O45" s="44"/>
+      <c r="P45" s="44"/>
+      <c r="Q45" s="44"/>
+      <c r="R45" s="44"/>
+      <c r="S45" s="44"/>
+      <c r="T45" s="44"/>
+      <c r="U45" s="44"/>
+      <c r="V45" s="44"/>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B46" s="37">
+        <v>3118410492</v>
+      </c>
+      <c r="C46" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="D45" s="73"/>
-      <c r="E45" s="73"/>
-      <c r="F45" s="73"/>
-      <c r="G45" s="73"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
-      <c r="K45" s="52"/>
-      <c r="L45" s="52"/>
-      <c r="M45" s="52"/>
-      <c r="N45" s="52"/>
-      <c r="O45" s="52"/>
-      <c r="P45" s="52"/>
-      <c r="Q45" s="52"/>
-      <c r="R45" s="52"/>
-      <c r="S45" s="52"/>
-      <c r="T45" s="52"/>
-      <c r="U45" s="52"/>
-      <c r="V45" s="52"/>
-    </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B46" s="44">
-        <v>3118410492</v>
-      </c>
-      <c r="C46" s="73" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="73"/>
-      <c r="G46" s="73"/>
-      <c r="H46" s="52"/>
-      <c r="I46" s="52"/>
-      <c r="J46" s="52"/>
-      <c r="K46" s="52"/>
-      <c r="L46" s="52"/>
-      <c r="M46" s="52"/>
-      <c r="N46" s="52"/>
-      <c r="O46" s="52"/>
-      <c r="P46" s="52"/>
-      <c r="Q46" s="52"/>
-      <c r="R46" s="52"/>
-      <c r="S46" s="52"/>
-      <c r="T46" s="52"/>
-      <c r="U46" s="52"/>
-      <c r="V46" s="52"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="52"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="44"/>
+      <c r="L46" s="44"/>
+      <c r="M46" s="44"/>
+      <c r="N46" s="44"/>
+      <c r="O46" s="44"/>
+      <c r="P46" s="44"/>
+      <c r="Q46" s="44"/>
+      <c r="R46" s="44"/>
+      <c r="S46" s="44"/>
+      <c r="T46" s="44"/>
+      <c r="U46" s="44"/>
+      <c r="V46" s="44"/>
     </row>
     <row r="49" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="43"/>
-      <c r="M49" s="43"/>
-      <c r="N49" s="43"/>
-      <c r="O49" s="43"/>
-      <c r="P49" s="43"/>
-      <c r="Q49" s="43"/>
-      <c r="R49" s="43"/>
-      <c r="S49" s="43"/>
-      <c r="T49" s="43"/>
-      <c r="U49" s="43"/>
-      <c r="V49" s="43"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="48"/>
+      <c r="K49" s="48"/>
+      <c r="L49" s="48"/>
+      <c r="M49" s="48"/>
+      <c r="N49" s="48"/>
+      <c r="O49" s="48"/>
+      <c r="P49" s="48"/>
+      <c r="Q49" s="48"/>
+      <c r="R49" s="48"/>
+      <c r="S49" s="48"/>
+      <c r="T49" s="48"/>
+      <c r="U49" s="48"/>
+      <c r="V49" s="48"/>
     </row>
     <row r="59" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B59" s="51"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="52"/>
-      <c r="E59" s="52"/>
-      <c r="F59" s="52"/>
-      <c r="G59" s="52"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="44"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="44"/>
     </row>
     <row r="60" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B60" s="51"/>
-      <c r="C60" s="52"/>
-      <c r="D60" s="52"/>
-      <c r="E60" s="52"/>
-      <c r="F60" s="52"/>
-      <c r="G60" s="52"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="44"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="44"/>
+      <c r="G60" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="75">
+  <mergeCells count="76">
+    <mergeCell ref="BL4:BR4"/>
+    <mergeCell ref="I1:Z1"/>
+    <mergeCell ref="AJ4:AP4"/>
+    <mergeCell ref="AQ4:AW4"/>
+    <mergeCell ref="AX4:BD4"/>
+    <mergeCell ref="BE4:BK4"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H4:N4"/>
+    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="V4:AB4"/>
+    <mergeCell ref="AC4:AI4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="H42:V42"/>
+    <mergeCell ref="H43:V43"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="H32:V32"/>
+    <mergeCell ref="H33:V33"/>
+    <mergeCell ref="H34:V34"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H35:V35"/>
+    <mergeCell ref="H40:V40"/>
+    <mergeCell ref="H41:V41"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H26:V26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H49:V49"/>
+    <mergeCell ref="H21:V21"/>
+    <mergeCell ref="H22:V22"/>
+    <mergeCell ref="H23:V23"/>
+    <mergeCell ref="H24:V24"/>
+    <mergeCell ref="H25:V25"/>
+    <mergeCell ref="H27:V27"/>
+    <mergeCell ref="H28:V28"/>
+    <mergeCell ref="H29:V29"/>
+    <mergeCell ref="H30:V30"/>
+    <mergeCell ref="H31:V31"/>
+    <mergeCell ref="H44:V44"/>
+    <mergeCell ref="H46:V46"/>
+    <mergeCell ref="H45:V45"/>
     <mergeCell ref="C60:G60"/>
     <mergeCell ref="C41:G41"/>
     <mergeCell ref="C21:G21"/>
@@ -3781,65 +4054,6 @@
     <mergeCell ref="C45:G45"/>
     <mergeCell ref="C46:G46"/>
     <mergeCell ref="C59:G59"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H49:V49"/>
-    <mergeCell ref="H21:V21"/>
-    <mergeCell ref="H22:V22"/>
-    <mergeCell ref="H23:V23"/>
-    <mergeCell ref="H24:V24"/>
-    <mergeCell ref="H25:V25"/>
-    <mergeCell ref="H27:V27"/>
-    <mergeCell ref="H28:V28"/>
-    <mergeCell ref="H29:V29"/>
-    <mergeCell ref="H30:V30"/>
-    <mergeCell ref="H31:V31"/>
-    <mergeCell ref="H44:V44"/>
-    <mergeCell ref="H46:V46"/>
-    <mergeCell ref="H45:V45"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H35:V35"/>
-    <mergeCell ref="H40:V40"/>
-    <mergeCell ref="H41:V41"/>
-    <mergeCell ref="H42:V42"/>
-    <mergeCell ref="H43:V43"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="H32:V32"/>
-    <mergeCell ref="H33:V33"/>
-    <mergeCell ref="H34:V34"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H26:V26"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H4:N4"/>
-    <mergeCell ref="O4:U4"/>
-    <mergeCell ref="V4:AB4"/>
-    <mergeCell ref="AC4:AI4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I1:Z1"/>
-    <mergeCell ref="AJ4:AP4"/>
-    <mergeCell ref="AQ4:AW4"/>
-    <mergeCell ref="AX4:BD4"/>
-    <mergeCell ref="BE4:BK4"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="D7:D19">
@@ -3856,7 +4070,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:BK19">
+  <conditionalFormatting sqref="H7:BR19">
     <cfRule type="expression" dxfId="2" priority="25">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
@@ -3864,7 +4078,7 @@
       <formula>AND(task_end&gt;=H$5,task_start&lt;H$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BK19">
+  <conditionalFormatting sqref="H5:BR19">
     <cfRule type="expression" dxfId="0" priority="27">
       <formula>AND(today&gt;=H$5,today&lt;H$5+1)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update activity bar chart
</commit_message>
<xml_diff>
--- a/Activity Bar Chart.xlsx
+++ b/Activity Bar Chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\quanlythuvien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4CA899-6934-45D1-8D82-FE2167FB41F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA05F67-629A-4C2A-9BB2-B356E7197C90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>Task 3</t>
   </si>
@@ -182,39 +182,18 @@
     <t>Vẽ demo giao diện GUI</t>
   </si>
   <si>
-    <t>Form sửa trạng thái mượn, trả sách</t>
-  </si>
-  <si>
-    <t>Form Thêm, sửa, xóa nhân viên</t>
-  </si>
-  <si>
-    <t>Form Thêm, sửa, xóa độc giả</t>
-  </si>
-  <si>
-    <t>Form Thêm, sửa, xóa sách</t>
-  </si>
-  <si>
-    <t>Form Tìm kiếm nhân viên, sách, độc giả</t>
-  </si>
-  <si>
     <t>Mã số sinh viên</t>
   </si>
   <si>
     <t>Tên sinh viên</t>
   </si>
   <si>
-    <t>Hiển thị danh sách sách mượn, tra cứu sách</t>
-  </si>
-  <si>
     <t>Nguyễn Quốc Khánh</t>
   </si>
   <si>
     <t>Nguyễn Quốc Tuấn</t>
   </si>
   <si>
-    <t>Nguyễn Khánh Ly</t>
-  </si>
-  <si>
     <t>Dương Khánh Ly</t>
   </si>
   <si>
@@ -230,13 +209,43 @@
     <t>Vũ Thị Hồng Xương</t>
   </si>
   <si>
-    <t>Xử lý phân quyền</t>
-  </si>
-  <si>
     <t>Form thống kê tình trạng sách(còn,mượn,trễ hẹn)</t>
   </si>
   <si>
     <t>Tạo database</t>
+  </si>
+  <si>
+    <t>Form Thêm, sửa, xóa,tìm kiếm sách</t>
+  </si>
+  <si>
+    <t>Form Thêm, sửa, xóa nhân viên,tìm kiếm</t>
+  </si>
+  <si>
+    <t>Form Quản lý mượn sách</t>
+  </si>
+  <si>
+    <t>Form đăng nhập</t>
+  </si>
+  <si>
+    <t>Form Quản lý nhập hàng</t>
+  </si>
+  <si>
+    <t>Task 14</t>
+  </si>
+  <si>
+    <t>Task 15</t>
+  </si>
+  <si>
+    <t>Form Quản lý thẻ đọc giả</t>
+  </si>
+  <si>
+    <t>Form Thêm, sửa, xóa,tìm kiếm đọc giả</t>
+  </si>
+  <si>
+    <t>Form Quản lý trả sách</t>
+  </si>
+  <si>
+    <t>Form Quản lý mức phạt</t>
   </si>
 </sst>
 </file>
@@ -823,7 +832,7 @@
     <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -928,7 +937,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="25" fillId="6" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -940,46 +948,13 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="24" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="25" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="26" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1001,23 +976,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="24" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="25" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="26" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1578,11 +1619,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BR60"/>
+  <dimension ref="A1:BR61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BL9" sqref="BL9"/>
+      <pane ySplit="6" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1602,32 +1643,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:70" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="43"/>
+      <c r="C1" s="42"/>
       <c r="D1" s="21"/>
       <c r="E1" s="2"/>
       <c r="F1" s="32"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="74"/>
-      <c r="X1" s="74"/>
-      <c r="Y1" s="74"/>
-      <c r="Z1" s="74"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
     </row>
     <row r="2" spans="1:70" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="36" t="s">
@@ -1637,20 +1678,20 @@
       <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="69">
+      <c r="E2" s="61">
         <v>44113</v>
       </c>
-      <c r="F2" s="70"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:70" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7"/>
       <c r="D3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="69">
+      <c r="E3" s="61">
         <v>44170</v>
       </c>
-      <c r="F3" s="70"/>
+      <c r="F3" s="62"/>
     </row>
     <row r="4" spans="1:70" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="4" t="s">
@@ -1659,96 +1700,96 @@
       <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="H4" s="71">
+      <c r="H4" s="57">
         <f>H5</f>
         <v>44109</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="71">
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="57">
         <f>O5</f>
         <v>44116</v>
       </c>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="72"/>
-      <c r="S4" s="72"/>
-      <c r="T4" s="72"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="71">
+      <c r="P4" s="58"/>
+      <c r="Q4" s="58"/>
+      <c r="R4" s="58"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="57">
         <f>V5</f>
         <v>44123</v>
       </c>
-      <c r="W4" s="72"/>
-      <c r="X4" s="72"/>
-      <c r="Y4" s="72"/>
-      <c r="Z4" s="72"/>
-      <c r="AA4" s="72"/>
-      <c r="AB4" s="73"/>
-      <c r="AC4" s="71">
+      <c r="W4" s="58"/>
+      <c r="X4" s="58"/>
+      <c r="Y4" s="58"/>
+      <c r="Z4" s="58"/>
+      <c r="AA4" s="58"/>
+      <c r="AB4" s="59"/>
+      <c r="AC4" s="57">
         <f>AC5</f>
         <v>44130</v>
       </c>
-      <c r="AD4" s="72"/>
-      <c r="AE4" s="72"/>
-      <c r="AF4" s="72"/>
-      <c r="AG4" s="72"/>
-      <c r="AH4" s="72"/>
-      <c r="AI4" s="73"/>
-      <c r="AJ4" s="71">
+      <c r="AD4" s="58"/>
+      <c r="AE4" s="58"/>
+      <c r="AF4" s="58"/>
+      <c r="AG4" s="58"/>
+      <c r="AH4" s="58"/>
+      <c r="AI4" s="59"/>
+      <c r="AJ4" s="57">
         <f>AJ5</f>
         <v>44137</v>
       </c>
-      <c r="AK4" s="72"/>
-      <c r="AL4" s="72"/>
-      <c r="AM4" s="72"/>
-      <c r="AN4" s="72"/>
-      <c r="AO4" s="72"/>
-      <c r="AP4" s="73"/>
-      <c r="AQ4" s="71">
+      <c r="AK4" s="58"/>
+      <c r="AL4" s="58"/>
+      <c r="AM4" s="58"/>
+      <c r="AN4" s="58"/>
+      <c r="AO4" s="58"/>
+      <c r="AP4" s="59"/>
+      <c r="AQ4" s="57">
         <f>AQ5</f>
         <v>44144</v>
       </c>
-      <c r="AR4" s="72"/>
-      <c r="AS4" s="72"/>
-      <c r="AT4" s="72"/>
-      <c r="AU4" s="72"/>
-      <c r="AV4" s="72"/>
-      <c r="AW4" s="73"/>
-      <c r="AX4" s="71">
+      <c r="AR4" s="58"/>
+      <c r="AS4" s="58"/>
+      <c r="AT4" s="58"/>
+      <c r="AU4" s="58"/>
+      <c r="AV4" s="58"/>
+      <c r="AW4" s="59"/>
+      <c r="AX4" s="57">
         <f>AX5</f>
         <v>44151</v>
       </c>
-      <c r="AY4" s="72"/>
-      <c r="AZ4" s="72"/>
-      <c r="BA4" s="72"/>
-      <c r="BB4" s="72"/>
-      <c r="BC4" s="72"/>
-      <c r="BD4" s="73"/>
-      <c r="BE4" s="71">
+      <c r="AY4" s="58"/>
+      <c r="AZ4" s="58"/>
+      <c r="BA4" s="58"/>
+      <c r="BB4" s="58"/>
+      <c r="BC4" s="58"/>
+      <c r="BD4" s="59"/>
+      <c r="BE4" s="57">
         <f>BE5</f>
         <v>44158</v>
       </c>
-      <c r="BF4" s="72"/>
-      <c r="BG4" s="72"/>
-      <c r="BH4" s="72"/>
-      <c r="BI4" s="72"/>
-      <c r="BJ4" s="72"/>
-      <c r="BK4" s="73"/>
-      <c r="BL4" s="71">
+      <c r="BF4" s="58"/>
+      <c r="BG4" s="58"/>
+      <c r="BH4" s="58"/>
+      <c r="BI4" s="58"/>
+      <c r="BJ4" s="58"/>
+      <c r="BK4" s="59"/>
+      <c r="BL4" s="57">
         <f>BL5</f>
         <v>44165</v>
       </c>
-      <c r="BM4" s="72"/>
-      <c r="BN4" s="72"/>
-      <c r="BO4" s="72"/>
-      <c r="BP4" s="72"/>
-      <c r="BQ4" s="72"/>
-      <c r="BR4" s="73"/>
+      <c r="BM4" s="58"/>
+      <c r="BN4" s="58"/>
+      <c r="BO4" s="58"/>
+      <c r="BP4" s="58"/>
+      <c r="BQ4" s="58"/>
+      <c r="BR4" s="59"/>
     </row>
     <row r="5" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
@@ -2018,10 +2059,10 @@
       <c r="E6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="F6" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="59"/>
+      <c r="G6" s="70"/>
       <c r="H6" s="13" t="str">
         <f t="shared" ref="H6" si="8">LEFT(TEXT(H5,"ddd"),1)</f>
         <v>M</v>
@@ -2167,7 +2208,7 @@
         <v>M</v>
       </c>
       <c r="AR6" s="13" t="str">
-        <f t="shared" ref="AR6:BL6" si="10">LEFT(TEXT(AR5,"ddd"),1)</f>
+        <f t="shared" ref="AR6:BK6" si="10">LEFT(TEXT(AR5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="AS6" s="13" t="str">
@@ -2285,10 +2326,10 @@
       <c r="E7" s="35">
         <v>44113</v>
       </c>
-      <c r="F7" s="53">
+      <c r="F7" s="67">
         <v>44113</v>
       </c>
-      <c r="G7" s="54"/>
+      <c r="G7" s="68"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
@@ -2363,10 +2404,10 @@
       <c r="E8" s="35">
         <v>44113</v>
       </c>
-      <c r="F8" s="53">
+      <c r="F8" s="67">
         <v>44114</v>
       </c>
-      <c r="G8" s="54"/>
+      <c r="G8" s="68"/>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
@@ -2441,10 +2482,10 @@
       <c r="E9" s="35">
         <v>44169</v>
       </c>
-      <c r="F9" s="53">
+      <c r="F9" s="67">
         <v>44170</v>
       </c>
-      <c r="G9" s="54"/>
+      <c r="G9" s="68"/>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
@@ -2519,10 +2560,10 @@
       <c r="E10" s="35">
         <v>44169</v>
       </c>
-      <c r="F10" s="53">
+      <c r="F10" s="67">
         <v>44170</v>
       </c>
-      <c r="G10" s="54"/>
+      <c r="G10" s="68"/>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
@@ -2597,10 +2638,10 @@
       <c r="E11" s="35">
         <v>44169</v>
       </c>
-      <c r="F11" s="53">
+      <c r="F11" s="67">
         <v>44170</v>
       </c>
-      <c r="G11" s="54"/>
+      <c r="G11" s="68"/>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
@@ -2675,10 +2716,10 @@
       <c r="E12" s="35">
         <v>44169</v>
       </c>
-      <c r="F12" s="53">
+      <c r="F12" s="67">
         <v>44170</v>
       </c>
-      <c r="G12" s="54"/>
+      <c r="G12" s="68"/>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
@@ -2753,10 +2794,10 @@
       <c r="E13" s="35">
         <v>44169</v>
       </c>
-      <c r="F13" s="53">
+      <c r="F13" s="67">
         <v>44170</v>
       </c>
-      <c r="G13" s="54"/>
+      <c r="G13" s="68"/>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
@@ -2831,10 +2872,10 @@
       <c r="E14" s="35">
         <v>44169</v>
       </c>
-      <c r="F14" s="53">
+      <c r="F14" s="67">
         <v>44170</v>
       </c>
-      <c r="G14" s="54"/>
+      <c r="G14" s="68"/>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
@@ -2909,10 +2950,10 @@
       <c r="E15" s="35">
         <v>44169</v>
       </c>
-      <c r="F15" s="53">
+      <c r="F15" s="67">
         <v>44170</v>
       </c>
-      <c r="G15" s="54"/>
+      <c r="G15" s="68"/>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
@@ -2987,10 +3028,10 @@
       <c r="E16" s="35">
         <v>44169</v>
       </c>
-      <c r="F16" s="53">
+      <c r="F16" s="67">
         <v>44170</v>
       </c>
-      <c r="G16" s="54"/>
+      <c r="G16" s="68"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
@@ -3065,10 +3106,10 @@
       <c r="E17" s="35">
         <v>44169</v>
       </c>
-      <c r="F17" s="53">
+      <c r="F17" s="67">
         <v>44170</v>
       </c>
-      <c r="G17" s="54"/>
+      <c r="G17" s="68"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
@@ -3133,7 +3174,7 @@
       <c r="BQ17" s="18"/>
       <c r="BR17" s="18"/>
     </row>
-    <row r="18" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:70" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
         <v>32</v>
@@ -3143,10 +3184,10 @@
       <c r="E18" s="35">
         <v>44169</v>
       </c>
-      <c r="F18" s="53">
+      <c r="F18" s="67">
         <v>44170</v>
       </c>
-      <c r="G18" s="54"/>
+      <c r="G18" s="68"/>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
@@ -3211,7 +3252,7 @@
       <c r="BQ18" s="18"/>
       <c r="BR18" s="18"/>
     </row>
-    <row r="19" spans="1:70" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:70" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15" t="s">
         <v>33</v>
@@ -3221,10 +3262,10 @@
       <c r="E19" s="35">
         <v>44169</v>
       </c>
-      <c r="F19" s="53">
+      <c r="F19" s="67">
         <v>44170</v>
       </c>
-      <c r="G19" s="54"/>
+      <c r="G19" s="68"/>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
@@ -3289,774 +3330,958 @@
       <c r="BQ19" s="18"/>
       <c r="BR19" s="18"/>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="48"/>
-      <c r="P21" s="48"/>
-      <c r="Q21" s="48"/>
-      <c r="R21" s="48"/>
-      <c r="S21" s="48"/>
-      <c r="T21" s="48"/>
-      <c r="U21" s="48"/>
-      <c r="V21" s="48"/>
+    <row r="20" spans="1:70" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="85"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="35">
+        <v>44169</v>
+      </c>
+      <c r="F20" s="67">
+        <v>44170</v>
+      </c>
+      <c r="G20" s="68"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="18"/>
+      <c r="U20" s="18"/>
+      <c r="V20" s="18"/>
+      <c r="W20" s="18"/>
+      <c r="X20" s="18"/>
+      <c r="Y20" s="18"/>
+      <c r="Z20" s="18"/>
+      <c r="AA20" s="18"/>
+      <c r="AB20" s="18"/>
+      <c r="AC20" s="18"/>
+      <c r="AD20" s="18"/>
+      <c r="AE20" s="18"/>
+      <c r="AF20" s="18"/>
+      <c r="AG20" s="18"/>
+      <c r="AH20" s="18"/>
+      <c r="AI20" s="18"/>
+      <c r="AJ20" s="18"/>
+      <c r="AK20" s="18"/>
+      <c r="AL20" s="18"/>
+      <c r="AM20" s="18"/>
+      <c r="AN20" s="18"/>
+      <c r="AO20" s="18"/>
+      <c r="AP20" s="18"/>
+      <c r="AQ20" s="18"/>
+      <c r="AR20" s="18"/>
+      <c r="AS20" s="18"/>
+      <c r="AT20" s="18"/>
+      <c r="AU20" s="18"/>
+      <c r="AV20" s="18"/>
+      <c r="AW20" s="18"/>
+      <c r="AX20" s="18"/>
+      <c r="AY20" s="18"/>
+      <c r="AZ20" s="18"/>
+      <c r="BA20" s="18"/>
+      <c r="BB20" s="18"/>
+      <c r="BC20" s="18"/>
+      <c r="BD20" s="18"/>
+      <c r="BE20" s="18"/>
+      <c r="BF20" s="18"/>
+      <c r="BG20" s="18"/>
+      <c r="BH20" s="18"/>
+      <c r="BI20" s="18"/>
+      <c r="BJ20" s="18"/>
+      <c r="BK20" s="18"/>
+      <c r="BL20" s="18"/>
+      <c r="BM20" s="18"/>
+      <c r="BN20" s="18"/>
+      <c r="BO20" s="18"/>
+      <c r="BP20" s="18"/>
+      <c r="BQ20" s="18"/>
+      <c r="BR20" s="18"/>
+    </row>
+    <row r="21" spans="1:70" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="85"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="35">
+        <v>44169</v>
+      </c>
+      <c r="F21" s="67">
+        <v>44170</v>
+      </c>
+      <c r="G21" s="68"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+      <c r="V21" s="18"/>
+      <c r="W21" s="18"/>
+      <c r="X21" s="18"/>
+      <c r="Y21" s="18"/>
+      <c r="Z21" s="18"/>
+      <c r="AA21" s="18"/>
+      <c r="AB21" s="18"/>
+      <c r="AC21" s="18"/>
+      <c r="AD21" s="18"/>
+      <c r="AE21" s="18"/>
+      <c r="AF21" s="18"/>
+      <c r="AG21" s="18"/>
+      <c r="AH21" s="18"/>
+      <c r="AI21" s="18"/>
+      <c r="AJ21" s="18"/>
+      <c r="AK21" s="18"/>
+      <c r="AL21" s="18"/>
+      <c r="AM21" s="18"/>
+      <c r="AN21" s="18"/>
+      <c r="AO21" s="18"/>
+      <c r="AP21" s="18"/>
+      <c r="AQ21" s="18"/>
+      <c r="AR21" s="18"/>
+      <c r="AS21" s="18"/>
+      <c r="AT21" s="18"/>
+      <c r="AU21" s="18"/>
+      <c r="AV21" s="18"/>
+      <c r="AW21" s="18"/>
+      <c r="AX21" s="18"/>
+      <c r="AY21" s="18"/>
+      <c r="AZ21" s="18"/>
+      <c r="BA21" s="18"/>
+      <c r="BB21" s="18"/>
+      <c r="BC21" s="18"/>
+      <c r="BD21" s="18"/>
+      <c r="BE21" s="18"/>
+      <c r="BF21" s="18"/>
+      <c r="BG21" s="18"/>
+      <c r="BH21" s="18"/>
+      <c r="BI21" s="18"/>
+      <c r="BJ21" s="18"/>
+      <c r="BK21" s="18"/>
+      <c r="BL21" s="18"/>
+      <c r="BM21" s="18"/>
+      <c r="BN21" s="18"/>
+      <c r="BO21" s="18"/>
+      <c r="BP21" s="18"/>
+      <c r="BQ21" s="18"/>
+      <c r="BR21" s="18"/>
     </row>
     <row r="22" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="B22" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="I22" s="56"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="56"/>
-      <c r="O22" s="56"/>
-      <c r="P22" s="56"/>
-      <c r="Q22" s="56"/>
-      <c r="R22" s="56"/>
-      <c r="S22" s="56"/>
-      <c r="T22" s="56"/>
-      <c r="U22" s="56"/>
-      <c r="V22" s="57"/>
-    </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="B23" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="46"/>
-      <c r="P23" s="46"/>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="46"/>
-      <c r="S23" s="46"/>
-      <c r="T23" s="46"/>
-      <c r="U23" s="46"/>
-      <c r="V23" s="47"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="71"/>
+      <c r="L22" s="71"/>
+      <c r="M22" s="71"/>
+      <c r="N22" s="71"/>
+      <c r="O22" s="71"/>
+      <c r="P22" s="71"/>
+      <c r="Q22" s="71"/>
+      <c r="R22" s="71"/>
+      <c r="S22" s="71"/>
+      <c r="T22" s="71"/>
+      <c r="U22" s="71"/>
+      <c r="V22" s="71"/>
     </row>
     <row r="24" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B24" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="72" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="73"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="73"/>
+      <c r="M24" s="73"/>
+      <c r="N24" s="73"/>
+      <c r="O24" s="73"/>
+      <c r="P24" s="73"/>
+      <c r="Q24" s="73"/>
+      <c r="R24" s="73"/>
+      <c r="S24" s="73"/>
+      <c r="T24" s="73"/>
+      <c r="U24" s="73"/>
+      <c r="V24" s="74"/>
+    </row>
+    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B25" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
+      <c r="P25" s="44"/>
+      <c r="Q25" s="44"/>
+      <c r="R25" s="44"/>
+      <c r="S25" s="44"/>
+      <c r="T25" s="44"/>
+      <c r="U25" s="44"/>
+      <c r="V25" s="45"/>
+    </row>
+    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B26" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="45" t="s">
+      <c r="C26" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="45" t="s">
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="46"/>
-      <c r="P24" s="46"/>
-      <c r="Q24" s="46"/>
-      <c r="R24" s="46"/>
-      <c r="S24" s="46"/>
-      <c r="T24" s="46"/>
-      <c r="U24" s="46"/>
-      <c r="V24" s="47"/>
-    </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="B25" s="38" t="s">
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+      <c r="P26" s="44"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
+      <c r="T26" s="44"/>
+      <c r="U26" s="44"/>
+      <c r="V26" s="45"/>
+    </row>
+    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B27" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="45" t="s">
+      <c r="C27" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
+      <c r="P27" s="44"/>
+      <c r="Q27" s="44"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="44"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="44"/>
+      <c r="V27" s="45"/>
+    </row>
+    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B28" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="44"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="44"/>
+      <c r="P28" s="44"/>
+      <c r="Q28" s="44"/>
+      <c r="R28" s="44"/>
+      <c r="S28" s="44"/>
+      <c r="T28" s="44"/>
+      <c r="U28" s="44"/>
+      <c r="V28" s="45"/>
+    </row>
+    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B29" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="44"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="44"/>
+      <c r="Q29" s="44"/>
+      <c r="R29" s="44"/>
+      <c r="S29" s="44"/>
+      <c r="T29" s="44"/>
+      <c r="U29" s="44"/>
+      <c r="V29" s="45"/>
+    </row>
+    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B30" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="46"/>
+      <c r="H30" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="44"/>
+      <c r="Q30" s="44"/>
+      <c r="R30" s="44"/>
+      <c r="S30" s="44"/>
+      <c r="T30" s="44"/>
+      <c r="U30" s="44"/>
+      <c r="V30" s="45"/>
+    </row>
+    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B31" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="46"/>
-      <c r="P25" s="46"/>
-      <c r="Q25" s="46"/>
-      <c r="R25" s="46"/>
-      <c r="S25" s="46"/>
-      <c r="T25" s="46"/>
-      <c r="U25" s="46"/>
-      <c r="V25" s="47"/>
-    </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="B26" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="I26" s="46"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46"/>
-      <c r="L26" s="46"/>
-      <c r="M26" s="46"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="46"/>
-      <c r="P26" s="46"/>
-      <c r="Q26" s="46"/>
-      <c r="R26" s="46"/>
-      <c r="S26" s="46"/>
-      <c r="T26" s="46"/>
-      <c r="U26" s="46"/>
-      <c r="V26" s="47"/>
-    </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="B27" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="46"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="46"/>
-      <c r="N27" s="46"/>
-      <c r="O27" s="46"/>
-      <c r="P27" s="46"/>
-      <c r="Q27" s="46"/>
-      <c r="R27" s="46"/>
-      <c r="S27" s="46"/>
-      <c r="T27" s="46"/>
-      <c r="U27" s="46"/>
-      <c r="V27" s="47"/>
-    </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="B28" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="I28" s="46"/>
-      <c r="J28" s="46"/>
-      <c r="K28" s="46"/>
-      <c r="L28" s="46"/>
-      <c r="M28" s="46"/>
-      <c r="N28" s="46"/>
-      <c r="O28" s="46"/>
-      <c r="P28" s="46"/>
-      <c r="Q28" s="46"/>
-      <c r="R28" s="46"/>
-      <c r="S28" s="46"/>
-      <c r="T28" s="46"/>
-      <c r="U28" s="46"/>
-      <c r="V28" s="47"/>
-    </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="B29" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="46"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="46"/>
-      <c r="P29" s="46"/>
-      <c r="Q29" s="46"/>
-      <c r="R29" s="46"/>
-      <c r="S29" s="46"/>
-      <c r="T29" s="46"/>
-      <c r="U29" s="46"/>
-      <c r="V29" s="47"/>
-    </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="B30" s="38" t="s">
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="44"/>
+      <c r="M31" s="44"/>
+      <c r="N31" s="44"/>
+      <c r="O31" s="44"/>
+      <c r="P31" s="44"/>
+      <c r="Q31" s="44"/>
+      <c r="R31" s="44"/>
+      <c r="S31" s="44"/>
+      <c r="T31" s="44"/>
+      <c r="U31" s="44"/>
+      <c r="V31" s="45"/>
+    </row>
+    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="B32" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="46"/>
-      <c r="M30" s="46"/>
-      <c r="N30" s="46"/>
-      <c r="O30" s="46"/>
-      <c r="P30" s="46"/>
-      <c r="Q30" s="46"/>
-      <c r="R30" s="46"/>
-      <c r="S30" s="46"/>
-      <c r="T30" s="46"/>
-      <c r="U30" s="46"/>
-      <c r="V30" s="47"/>
-    </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="B31" s="38" t="s">
+      <c r="C32" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="44"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="44"/>
+      <c r="O32" s="44"/>
+      <c r="P32" s="44"/>
+      <c r="Q32" s="44"/>
+      <c r="R32" s="44"/>
+      <c r="S32" s="44"/>
+      <c r="T32" s="44"/>
+      <c r="U32" s="44"/>
+      <c r="V32" s="45"/>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="45" t="s">
+      <c r="C33" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="44"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="44"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="44"/>
+      <c r="Q33" s="44"/>
+      <c r="R33" s="44"/>
+      <c r="S33" s="44"/>
+      <c r="T33" s="44"/>
+      <c r="U33" s="44"/>
+      <c r="V33" s="45"/>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B34" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="46"/>
-      <c r="P31" s="46"/>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="46"/>
-      <c r="S31" s="46"/>
-      <c r="T31" s="46"/>
-      <c r="U31" s="46"/>
-      <c r="V31" s="47"/>
-    </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="B32" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="46"/>
-      <c r="N32" s="46"/>
-      <c r="O32" s="46"/>
-      <c r="P32" s="46"/>
-      <c r="Q32" s="46"/>
-      <c r="R32" s="46"/>
-      <c r="S32" s="46"/>
-      <c r="T32" s="46"/>
-      <c r="U32" s="46"/>
-      <c r="V32" s="47"/>
-    </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B33" s="38" t="s">
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="44"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="44"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="44"/>
+      <c r="Q34" s="44"/>
+      <c r="R34" s="44"/>
+      <c r="S34" s="44"/>
+      <c r="T34" s="44"/>
+      <c r="U34" s="44"/>
+      <c r="V34" s="45"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B35" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="45" t="s">
+      <c r="C35" s="51" t="s">
         <v>58</v>
-      </c>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="46"/>
-      <c r="P33" s="46"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="46"/>
-      <c r="S33" s="46"/>
-      <c r="T33" s="46"/>
-      <c r="U33" s="46"/>
-      <c r="V33" s="47"/>
-    </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B34" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="I34" s="61"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="61"/>
-      <c r="L34" s="61"/>
-      <c r="M34" s="61"/>
-      <c r="N34" s="61"/>
-      <c r="O34" s="61"/>
-      <c r="P34" s="61"/>
-      <c r="Q34" s="61"/>
-      <c r="R34" s="61"/>
-      <c r="S34" s="61"/>
-      <c r="T34" s="61"/>
-      <c r="U34" s="61"/>
-      <c r="V34" s="62"/>
-    </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B35" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="52" t="s">
-        <v>62</v>
       </c>
       <c r="D35" s="52"/>
       <c r="E35" s="52"/>
       <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="I35" s="52"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="52"/>
-      <c r="L35" s="52"/>
-      <c r="M35" s="52"/>
-      <c r="N35" s="52"/>
-      <c r="O35" s="52"/>
-      <c r="P35" s="52"/>
-      <c r="Q35" s="52"/>
-      <c r="R35" s="52"/>
-      <c r="S35" s="52"/>
-      <c r="T35" s="52"/>
-      <c r="U35" s="52"/>
-      <c r="V35" s="52"/>
-    </row>
-    <row r="36" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B37" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="51"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
+      <c r="M35" s="44"/>
+      <c r="N35" s="44"/>
+      <c r="O35" s="44"/>
+      <c r="P35" s="44"/>
+      <c r="Q35" s="44"/>
+      <c r="R35" s="44"/>
+      <c r="S35" s="44"/>
+      <c r="T35" s="44"/>
+      <c r="U35" s="44"/>
+      <c r="V35" s="45"/>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B36" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="49"/>
+      <c r="N36" s="49"/>
+      <c r="O36" s="49"/>
+      <c r="P36" s="49"/>
+      <c r="Q36" s="49"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="49"/>
+      <c r="T36" s="49"/>
+      <c r="U36" s="49"/>
+      <c r="V36" s="50"/>
+    </row>
+    <row r="37" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="78" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="79"/>
+      <c r="E37" s="79"/>
+      <c r="F37" s="79"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="I37" s="79"/>
+      <c r="J37" s="79"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="79"/>
+      <c r="M37" s="79"/>
+      <c r="N37" s="79"/>
+      <c r="O37" s="79"/>
+      <c r="P37" s="79"/>
+      <c r="Q37" s="79"/>
+      <c r="R37" s="79"/>
+      <c r="S37" s="79"/>
+      <c r="T37" s="79"/>
+      <c r="U37" s="79"/>
+      <c r="V37" s="80"/>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B38" s="37">
-        <v>3118410148</v>
-      </c>
-      <c r="C38" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46"/>
-      <c r="G38" s="47"/>
+      <c r="B38" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="78" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="79"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="78" t="s">
+        <v>49</v>
+      </c>
+      <c r="I38" s="79"/>
+      <c r="J38" s="79"/>
+      <c r="K38" s="79"/>
+      <c r="L38" s="79"/>
+      <c r="M38" s="79"/>
+      <c r="N38" s="79"/>
+      <c r="O38" s="79"/>
+      <c r="P38" s="79"/>
+      <c r="Q38" s="79"/>
+      <c r="R38" s="79"/>
+      <c r="S38" s="79"/>
+      <c r="T38" s="79"/>
+      <c r="U38" s="79"/>
+      <c r="V38" s="80"/>
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B39" s="37">
-        <v>3118410411</v>
-      </c>
-      <c r="C39" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="46"/>
-      <c r="G39" s="47"/>
-    </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B40" s="37">
-        <v>3118410188</v>
-      </c>
-      <c r="C40" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="44"/>
-      <c r="M40" s="44"/>
-      <c r="N40" s="44"/>
-      <c r="O40" s="44"/>
-      <c r="P40" s="44"/>
-      <c r="Q40" s="44"/>
-      <c r="R40" s="44"/>
-      <c r="S40" s="44"/>
-      <c r="T40" s="44"/>
-      <c r="U40" s="44"/>
-      <c r="V40" s="44"/>
+      <c r="B39" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="78" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="79"/>
+      <c r="E39" s="79"/>
+      <c r="F39" s="79"/>
+      <c r="G39" s="80"/>
+      <c r="H39" s="81" t="s">
+        <v>52</v>
+      </c>
+      <c r="I39" s="81"/>
+      <c r="J39" s="81"/>
+      <c r="K39" s="82"/>
+      <c r="L39" s="83"/>
+      <c r="M39" s="83"/>
+      <c r="N39" s="83"/>
+      <c r="O39" s="83"/>
+      <c r="P39" s="83"/>
+      <c r="Q39" s="83"/>
+      <c r="R39" s="83"/>
+      <c r="S39" s="83"/>
+      <c r="T39" s="83"/>
+      <c r="U39" s="83"/>
+      <c r="V39" s="84"/>
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B41" s="37">
-        <v>3118412034</v>
-      </c>
-      <c r="C41" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="44"/>
-      <c r="J41" s="44"/>
-      <c r="K41" s="44"/>
-      <c r="L41" s="44"/>
-      <c r="M41" s="44"/>
-      <c r="N41" s="44"/>
-      <c r="O41" s="44"/>
-      <c r="P41" s="44"/>
-      <c r="Q41" s="44"/>
-      <c r="R41" s="44"/>
-      <c r="S41" s="44"/>
-      <c r="T41" s="44"/>
-      <c r="U41" s="44"/>
-      <c r="V41" s="44"/>
+      <c r="B41" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="77"/>
+      <c r="H41" s="63"/>
+      <c r="I41" s="63"/>
+      <c r="J41" s="63"/>
+      <c r="K41" s="63"/>
+      <c r="L41" s="63"/>
+      <c r="M41" s="63"/>
+      <c r="N41" s="63"/>
+      <c r="O41" s="63"/>
+      <c r="P41" s="63"/>
+      <c r="Q41" s="63"/>
+      <c r="R41" s="63"/>
+      <c r="S41" s="63"/>
+      <c r="T41" s="63"/>
+      <c r="U41" s="63"/>
+      <c r="V41" s="63"/>
     </row>
     <row r="42" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B42" s="37">
-        <v>3118410462</v>
-      </c>
-      <c r="C42" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44"/>
-      <c r="K42" s="44"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="44"/>
-      <c r="N42" s="44"/>
-      <c r="O42" s="44"/>
-      <c r="P42" s="44"/>
-      <c r="Q42" s="44"/>
-      <c r="R42" s="44"/>
-      <c r="S42" s="44"/>
-      <c r="T42" s="44"/>
-      <c r="U42" s="44"/>
-      <c r="V42" s="44"/>
+        <v>3118410148</v>
+      </c>
+      <c r="C42" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" s="65"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="65"/>
+      <c r="G42" s="66"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="63"/>
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63"/>
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="63"/>
+      <c r="S42" s="63"/>
+      <c r="T42" s="63"/>
+      <c r="U42" s="63"/>
+      <c r="V42" s="63"/>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B43" s="37">
-        <v>3118412036</v>
-      </c>
-      <c r="C43" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43" s="52"/>
-      <c r="E43" s="52"/>
-      <c r="F43" s="52"/>
-      <c r="G43" s="52"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="44"/>
-      <c r="O43" s="44"/>
-      <c r="P43" s="44"/>
-      <c r="Q43" s="44"/>
-      <c r="R43" s="44"/>
-      <c r="S43" s="44"/>
-      <c r="T43" s="44"/>
-      <c r="U43" s="44"/>
-      <c r="V43" s="44"/>
+        <v>3118410411</v>
+      </c>
+      <c r="C43" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="65"/>
+      <c r="E43" s="65"/>
+      <c r="F43" s="65"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63"/>
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63"/>
+      <c r="O43" s="63"/>
+      <c r="P43" s="63"/>
+      <c r="Q43" s="63"/>
+      <c r="R43" s="63"/>
+      <c r="S43" s="63"/>
+      <c r="T43" s="63"/>
+      <c r="U43" s="63"/>
+      <c r="V43" s="63"/>
     </row>
     <row r="44" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B44" s="37">
-        <v>3118410407</v>
-      </c>
-      <c r="C44" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="D44" s="52"/>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="44"/>
-      <c r="L44" s="44"/>
-      <c r="M44" s="44"/>
-      <c r="N44" s="44"/>
-      <c r="O44" s="44"/>
-      <c r="P44" s="44"/>
-      <c r="Q44" s="44"/>
-      <c r="R44" s="44"/>
-      <c r="S44" s="44"/>
-      <c r="T44" s="44"/>
-      <c r="U44" s="44"/>
-      <c r="V44" s="44"/>
+        <v>3118410188</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="63"/>
+      <c r="K44" s="63"/>
+      <c r="L44" s="63"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="63"/>
+      <c r="O44" s="63"/>
+      <c r="P44" s="63"/>
+      <c r="Q44" s="63"/>
+      <c r="R44" s="63"/>
+      <c r="S44" s="63"/>
+      <c r="T44" s="63"/>
+      <c r="U44" s="63"/>
+      <c r="V44" s="63"/>
     </row>
     <row r="45" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B45" s="37">
-        <v>3118410397</v>
-      </c>
-      <c r="C45" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="D45" s="52"/>
-      <c r="E45" s="52"/>
-      <c r="F45" s="52"/>
-      <c r="G45" s="52"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="44"/>
-      <c r="L45" s="44"/>
-      <c r="M45" s="44"/>
-      <c r="N45" s="44"/>
-      <c r="O45" s="44"/>
-      <c r="P45" s="44"/>
-      <c r="Q45" s="44"/>
-      <c r="R45" s="44"/>
-      <c r="S45" s="44"/>
-      <c r="T45" s="44"/>
-      <c r="U45" s="44"/>
-      <c r="V45" s="44"/>
+        <v>3118412034</v>
+      </c>
+      <c r="C45" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="63"/>
+      <c r="I45" s="63"/>
+      <c r="J45" s="63"/>
+      <c r="K45" s="63"/>
+      <c r="L45" s="63"/>
+      <c r="M45" s="63"/>
+      <c r="N45" s="63"/>
+      <c r="O45" s="63"/>
+      <c r="P45" s="63"/>
+      <c r="Q45" s="63"/>
+      <c r="R45" s="63"/>
+      <c r="S45" s="63"/>
+      <c r="T45" s="63"/>
+      <c r="U45" s="63"/>
+      <c r="V45" s="63"/>
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B46" s="37">
+        <v>3118410462</v>
+      </c>
+      <c r="C46" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="63"/>
+      <c r="I46" s="63"/>
+      <c r="J46" s="63"/>
+      <c r="K46" s="63"/>
+      <c r="L46" s="63"/>
+      <c r="M46" s="63"/>
+      <c r="N46" s="63"/>
+      <c r="O46" s="63"/>
+      <c r="P46" s="63"/>
+      <c r="Q46" s="63"/>
+      <c r="R46" s="63"/>
+      <c r="S46" s="63"/>
+      <c r="T46" s="63"/>
+      <c r="U46" s="63"/>
+      <c r="V46" s="63"/>
+    </row>
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B47" s="37">
+        <v>3118412036</v>
+      </c>
+      <c r="C47" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="79"/>
+      <c r="E47" s="79"/>
+      <c r="F47" s="79"/>
+      <c r="G47" s="80"/>
+      <c r="H47" s="63"/>
+      <c r="I47" s="63"/>
+      <c r="J47" s="63"/>
+      <c r="K47" s="63"/>
+      <c r="L47" s="63"/>
+      <c r="M47" s="63"/>
+      <c r="N47" s="63"/>
+      <c r="O47" s="63"/>
+      <c r="P47" s="63"/>
+      <c r="Q47" s="63"/>
+      <c r="R47" s="63"/>
+      <c r="S47" s="63"/>
+      <c r="T47" s="63"/>
+      <c r="U47" s="63"/>
+      <c r="V47" s="63"/>
+    </row>
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B48" s="37">
+        <v>3118410407</v>
+      </c>
+      <c r="C48" s="78" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="79"/>
+      <c r="E48" s="79"/>
+      <c r="F48" s="79"/>
+      <c r="G48" s="80"/>
+    </row>
+    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B49" s="37">
+        <v>3118410397</v>
+      </c>
+      <c r="C49" s="78" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="79"/>
+      <c r="E49" s="79"/>
+      <c r="F49" s="79"/>
+      <c r="G49" s="80"/>
+    </row>
+    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B50" s="37">
         <v>3118410492</v>
       </c>
-      <c r="C46" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46" s="52"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="52"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
-      <c r="K46" s="44"/>
-      <c r="L46" s="44"/>
-      <c r="M46" s="44"/>
-      <c r="N46" s="44"/>
-      <c r="O46" s="44"/>
-      <c r="P46" s="44"/>
-      <c r="Q46" s="44"/>
-      <c r="R46" s="44"/>
-      <c r="S46" s="44"/>
-      <c r="T46" s="44"/>
-      <c r="U46" s="44"/>
-      <c r="V46" s="44"/>
-    </row>
-    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="H49" s="48"/>
-      <c r="I49" s="48"/>
-      <c r="J49" s="48"/>
-      <c r="K49" s="48"/>
-      <c r="L49" s="48"/>
-      <c r="M49" s="48"/>
-      <c r="N49" s="48"/>
-      <c r="O49" s="48"/>
-      <c r="P49" s="48"/>
-      <c r="Q49" s="48"/>
-      <c r="R49" s="48"/>
-      <c r="S49" s="48"/>
-      <c r="T49" s="48"/>
-      <c r="U49" s="48"/>
-      <c r="V49" s="48"/>
-    </row>
-    <row r="59" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B59" s="40"/>
-      <c r="C59" s="44"/>
-      <c r="D59" s="44"/>
-      <c r="E59" s="44"/>
-      <c r="F59" s="44"/>
-      <c r="G59" s="44"/>
+      <c r="C50" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="D50" s="82"/>
+      <c r="E50" s="83"/>
+      <c r="F50" s="83"/>
+      <c r="G50" s="84"/>
+      <c r="H50" s="71"/>
+      <c r="I50" s="71"/>
+      <c r="J50" s="71"/>
+      <c r="K50" s="71"/>
+      <c r="L50" s="71"/>
+      <c r="M50" s="71"/>
+      <c r="N50" s="71"/>
+      <c r="O50" s="71"/>
+      <c r="P50" s="71"/>
+      <c r="Q50" s="71"/>
+      <c r="R50" s="71"/>
+      <c r="S50" s="71"/>
+      <c r="T50" s="71"/>
+      <c r="U50" s="71"/>
+      <c r="V50" s="71"/>
     </row>
     <row r="60" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B60" s="40"/>
-      <c r="C60" s="44"/>
-      <c r="D60" s="44"/>
-      <c r="E60" s="44"/>
-      <c r="F60" s="44"/>
-      <c r="G60" s="44"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="63"/>
+      <c r="D60" s="63"/>
+      <c r="E60" s="63"/>
+      <c r="F60" s="63"/>
+      <c r="G60" s="63"/>
+    </row>
+    <row r="61" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B61" s="39"/>
+      <c r="C61" s="63"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="63"/>
+      <c r="F61" s="63"/>
+      <c r="G61" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="76">
+  <mergeCells count="53">
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="H37:V37"/>
+    <mergeCell ref="H38:V38"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="C61:G61"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="H50:V50"/>
+    <mergeCell ref="H22:V22"/>
+    <mergeCell ref="H24:V24"/>
+    <mergeCell ref="H45:V45"/>
+    <mergeCell ref="H47:V47"/>
+    <mergeCell ref="H46:V46"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H41:V41"/>
+    <mergeCell ref="H42:V42"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="H43:V43"/>
+    <mergeCell ref="H44:V44"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H4:N4"/>
+    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="V4:AB4"/>
+    <mergeCell ref="AC4:AI4"/>
+    <mergeCell ref="E3:F3"/>
     <mergeCell ref="BL4:BR4"/>
     <mergeCell ref="I1:Z1"/>
     <mergeCell ref="AJ4:AP4"/>
     <mergeCell ref="AQ4:AW4"/>
     <mergeCell ref="AX4:BD4"/>
     <mergeCell ref="BE4:BK4"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H4:N4"/>
-    <mergeCell ref="O4:U4"/>
-    <mergeCell ref="V4:AB4"/>
-    <mergeCell ref="AC4:AI4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="H42:V42"/>
-    <mergeCell ref="H43:V43"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="H32:V32"/>
-    <mergeCell ref="H33:V33"/>
-    <mergeCell ref="H34:V34"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H35:V35"/>
-    <mergeCell ref="H40:V40"/>
-    <mergeCell ref="H41:V41"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H26:V26"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H49:V49"/>
-    <mergeCell ref="H21:V21"/>
-    <mergeCell ref="H22:V22"/>
-    <mergeCell ref="H23:V23"/>
-    <mergeCell ref="H24:V24"/>
-    <mergeCell ref="H25:V25"/>
-    <mergeCell ref="H27:V27"/>
-    <mergeCell ref="H28:V28"/>
-    <mergeCell ref="H29:V29"/>
-    <mergeCell ref="H30:V30"/>
-    <mergeCell ref="H31:V31"/>
-    <mergeCell ref="H44:V44"/>
-    <mergeCell ref="H46:V46"/>
-    <mergeCell ref="H45:V45"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C59:G59"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="D7:D19">
+  <conditionalFormatting sqref="D7:D21">
     <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4070,7 +4295,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:BR19">
+  <conditionalFormatting sqref="H7:BR21">
     <cfRule type="expression" dxfId="2" priority="25">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
@@ -4078,7 +4303,7 @@
       <formula>AND(task_end&gt;=H$5,task_start&lt;H$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BR19">
+  <conditionalFormatting sqref="H5:BR21">
     <cfRule type="expression" dxfId="0" priority="27">
       <formula>AND(today&gt;=H$5,today&lt;H$5+1)</formula>
     </cfRule>
@@ -4107,7 +4332,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D19</xm:sqref>
+          <xm:sqref>D7:D21</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>